<commit_message>
SQL: $body$; neue Python-Datei 'Datenbankverbindung'; test_setUp_tearDown in 'Test'-Ordner verschoben
</commit_message>
<xml_diff>
--- a/src/main/2 insert Sozialversicherungsdaten/1 Krankenversicherungsbeitraege.xlsx
+++ b/src/main/2 insert Sozialversicherungsdaten/1 Krankenversicherungsbeitraege.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\main\insert Sozialversicherungsdaten\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\main\2 insert Sozialversicherungsdaten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2A5C3D3-7163-4E1C-9210-1ABC0D6FD23A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7018A80-E5ED-4993-BB0A-7666822873F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2292" yWindow="1752" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -43,9 +43,6 @@
     <t>Eintragungsdatum</t>
   </si>
   <si>
-    <t>15.12.2023</t>
-  </si>
-  <si>
     <t>ermäßigter Beitragssatz</t>
   </si>
   <si>
@@ -62,6 +59,9 @@
   </si>
   <si>
     <t xml:space="preserve">Jahresarbeitsentgeltgrenze GKV </t>
+  </si>
+  <si>
+    <t>01.01.2024</t>
   </si>
 </sst>
 </file>
@@ -393,7 +393,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -412,10 +412,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -436,18 +436,18 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2">
-        <v>72453.56</v>
+        <v>62100</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2">
-        <v>75683.12</v>
+        <v>69300</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -455,7 +455,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -488,17 +488,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>